<commit_message>
Integration for Step 7
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -31,6 +31,84 @@
   </si>
   <si>
     <t>Leonard Hofstadter</t>
+  </si>
+  <si>
+    <t>Contact 1 Email</t>
+  </si>
+  <si>
+    <t>Contact 2 Email</t>
+  </si>
+  <si>
+    <t>sheldon@contoso.com</t>
+  </si>
+  <si>
+    <t>leonard@example.com</t>
+  </si>
+  <si>
+    <t>sheldon@example.com</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>EnailText</t>
+  </si>
+  <si>
+    <t>Imported from Rapise Email 1</t>
+  </si>
+  <si>
+    <t>Email1.txt</t>
+  </si>
+  <si>
+    <t>Email1.txtEmail1.txt</t>
+  </si>
+  <si>
+    <t>Email Text</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>WebServiceEWS</t>
+  </si>
+  <si>
+    <t>Email2,txt</t>
+  </si>
+  <si>
+    <t>Leonard HofstadterLeonard Hofstadter</t>
+  </si>
+  <si>
+    <t>Emmy</t>
+  </si>
+  <si>
+    <t>emmy@example.com</t>
+  </si>
+  <si>
+    <t>Penny</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>amy@example.com</t>
+  </si>
+  <si>
+    <t>penny@example.com</t>
+  </si>
+  <si>
+    <t>Imported from Rapise Email 2</t>
+  </si>
+  <si>
+    <t>Email2.txt</t>
+  </si>
+  <si>
+    <t>Amy Fowler</t>
+  </si>
+  <si>
+    <t>Penny Hofstadter</t>
   </si>
 </sst>
 </file>
@@ -51,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2501">
+  <borders count="2591">
     <border>
       <left/>
       <right/>
@@ -2559,11 +2637,101 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2501">
+  <cellXfs count="2591">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -5065,6 +5233,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2498" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2499" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2500" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2501" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2502" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2503" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2504" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2505" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2506" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2507" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2508" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2509" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2510" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2511" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2512" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2513" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2514" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2515" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2516" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2517" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2518" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2519" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2520" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2521" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2522" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2523" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2524" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2525" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2526" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2527" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2528" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2529" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2530" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2531" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2532" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2533" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2534" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2535" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2536" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2537" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2538" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2539" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2540" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2541" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2542" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2543" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2544" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2545" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2546" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2547" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2548" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2549" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2550" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2551" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2552" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2553" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2554" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2555" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2556" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2557" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2558" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2559" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2560" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2561" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2562" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2563" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2564" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2565" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2566" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2567" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2568" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2569" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2570" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2571" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2572" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2573" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2574" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2575" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2576" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2577" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2578" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2579" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2580" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2581" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2582" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2583" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2584" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2585" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2586" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2587" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2588" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2589" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2590" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5087,10 +5345,18 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="H1" s="8"/>
       <c r="I1" s="9"/>
       <c r="J1" s="10"/>
@@ -5145,10 +5411,18 @@
       <c r="C2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
+      <c r="D2" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>14</v>
+      </c>
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
       <c r="J2" s="60"/>
@@ -5194,13 +5468,27 @@
       <c r="AX2" s="100"/>
     </row>
     <row r="3">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="107"/>
+      <c r="A3" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="103" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="106" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="107" t="s">
+        <v>29</v>
+      </c>
       <c r="H3" s="108"/>
       <c r="I3" s="109"/>
       <c r="J3" s="110"/>
@@ -5251,7 +5539,9 @@
       <c r="C4" s="153"/>
       <c r="D4" s="154"/>
       <c r="E4" s="155"/>
-      <c r="F4" s="156"/>
+      <c r="F4" s="156" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="157"/>
       <c r="H4" s="158"/>
       <c r="I4" s="159"/>

</xml_diff>